<commit_message>
First week's data and initial report code
</commit_message>
<xml_diff>
--- a/Data/raw_fecund_data.xlsx
+++ b/Data/raw_fecund_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/Lab_Projects/01_Small_projects/freshwater_choice/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1B63CC-675E-8A45-8829-0B6465665FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0376DC-805E-E54A-869A-ABBEBEC605BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{8320B239-817B-2D40-83A6-DE83587F0EE7}"/>
+    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{8320B239-817B-2D40-83A6-DE83587F0EE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="26">
   <si>
     <t>exp_rep</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>dropped</t>
+  </si>
+  <si>
+    <t>released</t>
   </si>
 </sst>
 </file>
@@ -468,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8949BF81-7D7A-4643-97D8-DBE58FB94094}">
-  <dimension ref="A1:R55"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,6 +551,24 @@
       <c r="E2">
         <v>8</v>
       </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -565,6 +586,24 @@
       <c r="E3">
         <v>5</v>
       </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -582,6 +621,24 @@
       <c r="E4">
         <v>11</v>
       </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -599,6 +656,24 @@
       <c r="E5">
         <v>5</v>
       </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -616,6 +691,24 @@
       <c r="E6">
         <v>10</v>
       </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -633,6 +726,24 @@
       <c r="E7">
         <v>8</v>
       </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -650,6 +761,24 @@
       <c r="E8">
         <v>10</v>
       </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -667,6 +796,24 @@
       <c r="E9">
         <v>10</v>
       </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -684,6 +831,24 @@
       <c r="E10">
         <v>12</v>
       </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -701,6 +866,24 @@
       <c r="E11">
         <v>12</v>
       </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -718,6 +901,24 @@
       <c r="E12">
         <v>12</v>
       </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -735,6 +936,24 @@
       <c r="E13">
         <v>18</v>
       </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -752,6 +971,24 @@
       <c r="E14" t="s">
         <v>23</v>
       </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -769,6 +1006,24 @@
       <c r="E15" t="s">
         <v>23</v>
       </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -786,8 +1041,26 @@
       <c r="E16">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -803,8 +1076,26 @@
       <c r="E17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -820,8 +1111,26 @@
       <c r="E18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -837,8 +1146,26 @@
       <c r="E19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -854,8 +1181,26 @@
       <c r="E20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -871,8 +1216,26 @@
       <c r="E21">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -888,8 +1251,26 @@
       <c r="E22">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -905,8 +1286,26 @@
       <c r="E23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -922,8 +1321,26 @@
       <c r="E24">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -939,8 +1356,26 @@
       <c r="E25">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -956,8 +1391,26 @@
       <c r="E26">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -973,8 +1426,26 @@
       <c r="E27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -990,8 +1461,26 @@
       <c r="E28">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1002,10 +1491,25 @@
         <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="E29">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -1016,10 +1520,25 @@
         <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" t="s">
+        <v>23</v>
+      </c>
+      <c r="I30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1030,10 +1549,25 @@
         <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="E31">
+        <v>12</v>
+      </c>
+      <c r="F31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -1044,10 +1578,25 @@
         <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1058,10 +1607,25 @@
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="E33">
+        <v>8</v>
+      </c>
+      <c r="F33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" t="s">
+        <v>23</v>
+      </c>
+      <c r="H33" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -1072,10 +1636,25 @@
         <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -1086,293 +1665,57 @@
         <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="E35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
       <c r="B36">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C36">
         <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37">
-        <v>9</v>
-      </c>
-      <c r="C37">
-        <v>20</v>
-      </c>
-      <c r="D37" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38">
-        <v>10</v>
-      </c>
-      <c r="C38">
-        <v>10</v>
-      </c>
-      <c r="D38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39">
-        <v>11</v>
-      </c>
-      <c r="C39">
-        <v>10</v>
-      </c>
-      <c r="D39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40">
+        <v>19</v>
+      </c>
+      <c r="E36">
         <v>12</v>
       </c>
-      <c r="C40">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41">
-        <v>13</v>
-      </c>
-      <c r="C41">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42">
-        <v>14</v>
-      </c>
-      <c r="C42">
-        <v>10</v>
-      </c>
-      <c r="D42" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43">
-        <v>15</v>
-      </c>
-      <c r="C43">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44">
-        <v>16</v>
-      </c>
-      <c r="C44">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45">
-        <v>17</v>
-      </c>
-      <c r="C45">
-        <v>10</v>
-      </c>
-      <c r="D45" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>22</v>
-      </c>
-      <c r="B46">
-        <v>18</v>
-      </c>
-      <c r="C46">
-        <v>10</v>
-      </c>
-      <c r="D46" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>22</v>
-      </c>
-      <c r="B47">
-        <v>19</v>
-      </c>
-      <c r="C47">
-        <v>10</v>
-      </c>
-      <c r="D47" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>22</v>
-      </c>
-      <c r="B48">
-        <v>20</v>
-      </c>
-      <c r="C48">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>22</v>
-      </c>
-      <c r="B49">
-        <v>21</v>
-      </c>
-      <c r="C49">
-        <v>10</v>
-      </c>
-      <c r="D49" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50">
-        <v>22</v>
-      </c>
-      <c r="C50">
-        <v>10</v>
-      </c>
-      <c r="D50" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>22</v>
-      </c>
-      <c r="B51">
-        <v>23</v>
-      </c>
-      <c r="C51">
-        <v>10</v>
-      </c>
-      <c r="D51" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>22</v>
-      </c>
-      <c r="B52">
+      <c r="F36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" t="s">
         <v>24</v>
       </c>
-      <c r="C52">
-        <v>10</v>
-      </c>
-      <c r="D52" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>22</v>
-      </c>
-      <c r="B53">
-        <v>25</v>
-      </c>
-      <c r="C53">
-        <v>10</v>
-      </c>
-      <c r="D53" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>22</v>
-      </c>
-      <c r="B54">
-        <v>26</v>
-      </c>
-      <c r="C54">
-        <v>10</v>
-      </c>
-      <c r="D54" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>22</v>
-      </c>
-      <c r="B55">
-        <v>27</v>
-      </c>
-      <c r="C55">
-        <v>10</v>
-      </c>
-      <c r="D55" t="s">
-        <v>19</v>
+      <c r="H36" t="s">
+        <v>23</v>
+      </c>
+      <c r="I36" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R55">
-    <sortCondition ref="A2:A55"/>
-    <sortCondition ref="B2:B55"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R54">
+    <sortCondition ref="A2:A54"/>
+    <sortCondition ref="B2:B54"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Data update and directory clean up
</commit_message>
<xml_diff>
--- a/Data/raw_fecund_data.xlsx
+++ b/Data/raw_fecund_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/Lab_Projects/01_Small_projects/freshwater_choice/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0376DC-805E-E54A-869A-ABBEBEC605BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D086B7-7DDF-CB42-AFC8-4316CF9EB6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{8320B239-817B-2D40-83A6-DE83587F0EE7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="26">
   <si>
     <t>exp_rep</t>
   </si>
@@ -473,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8949BF81-7D7A-4643-97D8-DBE58FB94094}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,6 +569,21 @@
       <c r="K2" t="s">
         <v>23</v>
       </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -604,6 +619,21 @@
       <c r="K3" t="s">
         <v>23</v>
       </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -639,6 +669,21 @@
       <c r="K4" t="s">
         <v>23</v>
       </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -674,6 +719,21 @@
       <c r="K5" t="s">
         <v>25</v>
       </c>
+      <c r="L5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -709,6 +769,21 @@
       <c r="K6" t="s">
         <v>23</v>
       </c>
+      <c r="L6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -744,6 +819,21 @@
       <c r="K7" t="s">
         <v>23</v>
       </c>
+      <c r="L7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -779,6 +869,21 @@
       <c r="K8" t="s">
         <v>23</v>
       </c>
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -814,6 +919,21 @@
       <c r="K9" t="s">
         <v>23</v>
       </c>
+      <c r="L9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -849,6 +969,21 @@
       <c r="K10" t="s">
         <v>25</v>
       </c>
+      <c r="L10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -884,6 +1019,21 @@
       <c r="K11" t="s">
         <v>23</v>
       </c>
+      <c r="L11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" t="s">
+        <v>23</v>
+      </c>
+      <c r="P11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -919,6 +1069,21 @@
       <c r="K12" t="s">
         <v>23</v>
       </c>
+      <c r="L12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" t="s">
+        <v>23</v>
+      </c>
+      <c r="P12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -954,6 +1119,21 @@
       <c r="K13" t="s">
         <v>23</v>
       </c>
+      <c r="L13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" t="s">
+        <v>23</v>
+      </c>
+      <c r="P13" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -989,6 +1169,21 @@
       <c r="K14" t="s">
         <v>23</v>
       </c>
+      <c r="L14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" t="s">
+        <v>23</v>
+      </c>
+      <c r="O14" t="s">
+        <v>23</v>
+      </c>
+      <c r="P14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1024,6 +1219,21 @@
       <c r="K15" t="s">
         <v>23</v>
       </c>
+      <c r="L15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1059,8 +1269,23 @@
       <c r="K16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" t="s">
+        <v>23</v>
+      </c>
+      <c r="O16" t="s">
+        <v>23</v>
+      </c>
+      <c r="P16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1094,8 +1319,23 @@
       <c r="K17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" t="s">
+        <v>23</v>
+      </c>
+      <c r="N17" t="s">
+        <v>23</v>
+      </c>
+      <c r="O17" t="s">
+        <v>23</v>
+      </c>
+      <c r="P17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1129,8 +1369,23 @@
       <c r="K18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M18" t="s">
+        <v>23</v>
+      </c>
+      <c r="N18" t="s">
+        <v>23</v>
+      </c>
+      <c r="O18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1164,8 +1419,23 @@
       <c r="K19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" t="s">
+        <v>23</v>
+      </c>
+      <c r="N19" t="s">
+        <v>23</v>
+      </c>
+      <c r="O19" t="s">
+        <v>23</v>
+      </c>
+      <c r="P19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1199,8 +1469,23 @@
       <c r="K20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M20" t="s">
+        <v>23</v>
+      </c>
+      <c r="N20" t="s">
+        <v>23</v>
+      </c>
+      <c r="O20" t="s">
+        <v>23</v>
+      </c>
+      <c r="P20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1234,8 +1519,23 @@
       <c r="K21" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21" t="s">
+        <v>23</v>
+      </c>
+      <c r="N21" t="s">
+        <v>23</v>
+      </c>
+      <c r="O21" t="s">
+        <v>23</v>
+      </c>
+      <c r="P21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1269,8 +1569,23 @@
       <c r="K22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22" t="s">
+        <v>23</v>
+      </c>
+      <c r="M22" t="s">
+        <v>23</v>
+      </c>
+      <c r="N22" t="s">
+        <v>23</v>
+      </c>
+      <c r="O22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1304,8 +1619,23 @@
       <c r="K23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" t="s">
+        <v>23</v>
+      </c>
+      <c r="N23" t="s">
+        <v>23</v>
+      </c>
+      <c r="O23" t="s">
+        <v>23</v>
+      </c>
+      <c r="P23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1339,8 +1669,23 @@
       <c r="K24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24" t="s">
+        <v>23</v>
+      </c>
+      <c r="M24" t="s">
+        <v>23</v>
+      </c>
+      <c r="N24" t="s">
+        <v>23</v>
+      </c>
+      <c r="O24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1374,8 +1719,23 @@
       <c r="K25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25" t="s">
+        <v>23</v>
+      </c>
+      <c r="M25" t="s">
+        <v>23</v>
+      </c>
+      <c r="N25" t="s">
+        <v>23</v>
+      </c>
+      <c r="O25" t="s">
+        <v>23</v>
+      </c>
+      <c r="P25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1409,8 +1769,23 @@
       <c r="K26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26" t="s">
+        <v>23</v>
+      </c>
+      <c r="M26" t="s">
+        <v>23</v>
+      </c>
+      <c r="N26" t="s">
+        <v>23</v>
+      </c>
+      <c r="O26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -1444,8 +1819,23 @@
       <c r="K27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27" t="s">
+        <v>23</v>
+      </c>
+      <c r="M27" t="s">
+        <v>23</v>
+      </c>
+      <c r="N27" t="s">
+        <v>23</v>
+      </c>
+      <c r="O27" t="s">
+        <v>23</v>
+      </c>
+      <c r="P27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1479,8 +1869,23 @@
       <c r="K28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28" t="s">
+        <v>23</v>
+      </c>
+      <c r="M28" t="s">
+        <v>23</v>
+      </c>
+      <c r="N28" t="s">
+        <v>23</v>
+      </c>
+      <c r="O28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1508,8 +1913,23 @@
       <c r="I29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29" t="s">
+        <v>23</v>
+      </c>
+      <c r="M29" t="s">
+        <v>23</v>
+      </c>
+      <c r="N29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -1537,8 +1957,23 @@
       <c r="I30" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J30" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" t="s">
+        <v>23</v>
+      </c>
+      <c r="L30" t="s">
+        <v>23</v>
+      </c>
+      <c r="M30" t="s">
+        <v>23</v>
+      </c>
+      <c r="N30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1566,8 +2001,23 @@
       <c r="I31" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J31" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31" t="s">
+        <v>23</v>
+      </c>
+      <c r="L31" t="s">
+        <v>23</v>
+      </c>
+      <c r="M31" t="s">
+        <v>23</v>
+      </c>
+      <c r="N31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -1595,8 +2045,23 @@
       <c r="I32" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" t="s">
+        <v>23</v>
+      </c>
+      <c r="L32" t="s">
+        <v>23</v>
+      </c>
+      <c r="M32" t="s">
+        <v>23</v>
+      </c>
+      <c r="N32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1624,8 +2089,23 @@
       <c r="I33" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" t="s">
+        <v>23</v>
+      </c>
+      <c r="K33" t="s">
+        <v>23</v>
+      </c>
+      <c r="L33" t="s">
+        <v>25</v>
+      </c>
+      <c r="M33" t="s">
+        <v>25</v>
+      </c>
+      <c r="N33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -1653,8 +2133,23 @@
       <c r="I34" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34" t="s">
+        <v>25</v>
+      </c>
+      <c r="K34" t="s">
+        <v>23</v>
+      </c>
+      <c r="L34" t="s">
+        <v>23</v>
+      </c>
+      <c r="M34" t="s">
+        <v>23</v>
+      </c>
+      <c r="N34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -1682,8 +2177,23 @@
       <c r="I35" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" t="s">
+        <v>23</v>
+      </c>
+      <c r="L35" t="s">
+        <v>23</v>
+      </c>
+      <c r="M35" t="s">
+        <v>23</v>
+      </c>
+      <c r="N35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1709,6 +2219,21 @@
         <v>23</v>
       </c>
       <c r="I36" t="s">
+        <v>23</v>
+      </c>
+      <c r="J36" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" t="s">
+        <v>23</v>
+      </c>
+      <c r="L36" t="s">
+        <v>23</v>
+      </c>
+      <c r="M36" t="s">
+        <v>23</v>
+      </c>
+      <c r="N36" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding first batch of size data and updating surv data.
</commit_message>
<xml_diff>
--- a/Data/raw_fecund_data.xlsx
+++ b/Data/raw_fecund_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/Lab_Projects/01_Small_projects/freshwater_choice/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D086B7-7DDF-CB42-AFC8-4316CF9EB6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B3C4ED-57E1-9A45-8976-C28CB2AC61EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{8320B239-817B-2D40-83A6-DE83587F0EE7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="32">
   <si>
     <t>exp_rep</t>
   </si>
@@ -114,6 +114,24 @@
   </si>
   <si>
     <t>released</t>
+  </si>
+  <si>
+    <t>day15</t>
+  </si>
+  <si>
+    <t>day16</t>
+  </si>
+  <si>
+    <t>day17</t>
+  </si>
+  <si>
+    <t>day18</t>
+  </si>
+  <si>
+    <t>day19</t>
+  </si>
+  <si>
+    <t>day20</t>
   </si>
 </sst>
 </file>
@@ -471,15 +489,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8949BF81-7D7A-4643-97D8-DBE58FB94094}">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V29" sqref="V29:V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -534,8 +552,26 @@
       <c r="R1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -584,8 +620,32 @@
       <c r="P2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" t="s">
+        <v>23</v>
+      </c>
+      <c r="V2" t="s">
+        <v>23</v>
+      </c>
+      <c r="W2" t="s">
+        <v>23</v>
+      </c>
+      <c r="X2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -634,8 +694,32 @@
       <c r="P3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U3" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" t="s">
+        <v>23</v>
+      </c>
+      <c r="W3" t="s">
+        <v>23</v>
+      </c>
+      <c r="X3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -684,8 +768,32 @@
       <c r="P4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" t="s">
+        <v>23</v>
+      </c>
+      <c r="U4" t="s">
+        <v>23</v>
+      </c>
+      <c r="V4" t="s">
+        <v>23</v>
+      </c>
+      <c r="W4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -734,8 +842,32 @@
       <c r="P5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V5" t="s">
+        <v>23</v>
+      </c>
+      <c r="W5" t="s">
+        <v>23</v>
+      </c>
+      <c r="X5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -784,8 +916,32 @@
       <c r="P6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S6" t="s">
+        <v>23</v>
+      </c>
+      <c r="T6" t="s">
+        <v>23</v>
+      </c>
+      <c r="U6" t="s">
+        <v>23</v>
+      </c>
+      <c r="V6" t="s">
+        <v>23</v>
+      </c>
+      <c r="W6" t="s">
+        <v>23</v>
+      </c>
+      <c r="X6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -834,8 +990,32 @@
       <c r="P7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R7" t="s">
+        <v>23</v>
+      </c>
+      <c r="S7" t="s">
+        <v>23</v>
+      </c>
+      <c r="T7" t="s">
+        <v>23</v>
+      </c>
+      <c r="U7" t="s">
+        <v>23</v>
+      </c>
+      <c r="V7" t="s">
+        <v>23</v>
+      </c>
+      <c r="W7" t="s">
+        <v>23</v>
+      </c>
+      <c r="X7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -884,8 +1064,32 @@
       <c r="P8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q8" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S8" t="s">
+        <v>23</v>
+      </c>
+      <c r="T8" t="s">
+        <v>23</v>
+      </c>
+      <c r="U8" t="s">
+        <v>23</v>
+      </c>
+      <c r="V8" t="s">
+        <v>23</v>
+      </c>
+      <c r="W8" t="s">
+        <v>23</v>
+      </c>
+      <c r="X8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -934,8 +1138,32 @@
       <c r="P9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q9" t="s">
+        <v>23</v>
+      </c>
+      <c r="R9" t="s">
+        <v>23</v>
+      </c>
+      <c r="S9" t="s">
+        <v>23</v>
+      </c>
+      <c r="T9" t="s">
+        <v>23</v>
+      </c>
+      <c r="U9" t="s">
+        <v>23</v>
+      </c>
+      <c r="V9" t="s">
+        <v>23</v>
+      </c>
+      <c r="W9" t="s">
+        <v>23</v>
+      </c>
+      <c r="X9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -984,8 +1212,32 @@
       <c r="P10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q10" t="s">
+        <v>23</v>
+      </c>
+      <c r="R10" t="s">
+        <v>23</v>
+      </c>
+      <c r="S10" t="s">
+        <v>23</v>
+      </c>
+      <c r="T10" t="s">
+        <v>23</v>
+      </c>
+      <c r="U10" t="s">
+        <v>23</v>
+      </c>
+      <c r="V10" t="s">
+        <v>23</v>
+      </c>
+      <c r="W10" t="s">
+        <v>23</v>
+      </c>
+      <c r="X10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1034,8 +1286,32 @@
       <c r="P11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q11" t="s">
+        <v>23</v>
+      </c>
+      <c r="R11" t="s">
+        <v>23</v>
+      </c>
+      <c r="S11" t="s">
+        <v>23</v>
+      </c>
+      <c r="T11" t="s">
+        <v>23</v>
+      </c>
+      <c r="U11" t="s">
+        <v>23</v>
+      </c>
+      <c r="V11" t="s">
+        <v>23</v>
+      </c>
+      <c r="W11" t="s">
+        <v>23</v>
+      </c>
+      <c r="X11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1084,8 +1360,32 @@
       <c r="P12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q12" t="s">
+        <v>23</v>
+      </c>
+      <c r="R12" t="s">
+        <v>23</v>
+      </c>
+      <c r="S12" t="s">
+        <v>23</v>
+      </c>
+      <c r="T12" t="s">
+        <v>23</v>
+      </c>
+      <c r="U12" t="s">
+        <v>23</v>
+      </c>
+      <c r="V12" t="s">
+        <v>23</v>
+      </c>
+      <c r="W12" t="s">
+        <v>23</v>
+      </c>
+      <c r="X12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1134,8 +1434,32 @@
       <c r="P13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q13" t="s">
+        <v>23</v>
+      </c>
+      <c r="R13" t="s">
+        <v>23</v>
+      </c>
+      <c r="S13" t="s">
+        <v>23</v>
+      </c>
+      <c r="T13" t="s">
+        <v>23</v>
+      </c>
+      <c r="U13" t="s">
+        <v>23</v>
+      </c>
+      <c r="V13" t="s">
+        <v>23</v>
+      </c>
+      <c r="W13" t="s">
+        <v>23</v>
+      </c>
+      <c r="X13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1184,8 +1508,32 @@
       <c r="P14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q14" t="s">
+        <v>23</v>
+      </c>
+      <c r="R14" t="s">
+        <v>23</v>
+      </c>
+      <c r="S14" t="s">
+        <v>23</v>
+      </c>
+      <c r="T14" t="s">
+        <v>23</v>
+      </c>
+      <c r="U14" t="s">
+        <v>23</v>
+      </c>
+      <c r="V14" t="s">
+        <v>23</v>
+      </c>
+      <c r="W14" t="s">
+        <v>23</v>
+      </c>
+      <c r="X14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1234,8 +1582,32 @@
       <c r="P15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q15" t="s">
+        <v>23</v>
+      </c>
+      <c r="R15" t="s">
+        <v>23</v>
+      </c>
+      <c r="S15" t="s">
+        <v>23</v>
+      </c>
+      <c r="T15" t="s">
+        <v>23</v>
+      </c>
+      <c r="U15" t="s">
+        <v>23</v>
+      </c>
+      <c r="V15" t="s">
+        <v>23</v>
+      </c>
+      <c r="W15" t="s">
+        <v>23</v>
+      </c>
+      <c r="X15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1284,8 +1656,32 @@
       <c r="P16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q16" t="s">
+        <v>23</v>
+      </c>
+      <c r="R16" t="s">
+        <v>23</v>
+      </c>
+      <c r="S16" t="s">
+        <v>23</v>
+      </c>
+      <c r="T16" t="s">
+        <v>23</v>
+      </c>
+      <c r="U16" t="s">
+        <v>23</v>
+      </c>
+      <c r="V16" t="s">
+        <v>23</v>
+      </c>
+      <c r="W16" t="s">
+        <v>23</v>
+      </c>
+      <c r="X16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1334,8 +1730,32 @@
       <c r="P17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q17" t="s">
+        <v>23</v>
+      </c>
+      <c r="R17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S17" t="s">
+        <v>23</v>
+      </c>
+      <c r="T17" t="s">
+        <v>23</v>
+      </c>
+      <c r="U17" t="s">
+        <v>23</v>
+      </c>
+      <c r="V17" t="s">
+        <v>23</v>
+      </c>
+      <c r="W17" t="s">
+        <v>23</v>
+      </c>
+      <c r="X17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1384,8 +1804,32 @@
       <c r="P18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q18" t="s">
+        <v>23</v>
+      </c>
+      <c r="R18" t="s">
+        <v>23</v>
+      </c>
+      <c r="S18" t="s">
+        <v>23</v>
+      </c>
+      <c r="T18" t="s">
+        <v>23</v>
+      </c>
+      <c r="U18" t="s">
+        <v>23</v>
+      </c>
+      <c r="V18" t="s">
+        <v>23</v>
+      </c>
+      <c r="W18" t="s">
+        <v>23</v>
+      </c>
+      <c r="X18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1434,8 +1878,32 @@
       <c r="P19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q19" t="s">
+        <v>23</v>
+      </c>
+      <c r="R19" t="s">
+        <v>23</v>
+      </c>
+      <c r="S19" t="s">
+        <v>23</v>
+      </c>
+      <c r="T19" t="s">
+        <v>23</v>
+      </c>
+      <c r="U19" t="s">
+        <v>23</v>
+      </c>
+      <c r="V19" t="s">
+        <v>23</v>
+      </c>
+      <c r="W19" t="s">
+        <v>23</v>
+      </c>
+      <c r="X19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1484,8 +1952,32 @@
       <c r="P20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q20" t="s">
+        <v>23</v>
+      </c>
+      <c r="R20" t="s">
+        <v>23</v>
+      </c>
+      <c r="S20" t="s">
+        <v>23</v>
+      </c>
+      <c r="T20" t="s">
+        <v>23</v>
+      </c>
+      <c r="U20" t="s">
+        <v>23</v>
+      </c>
+      <c r="V20" t="s">
+        <v>23</v>
+      </c>
+      <c r="W20" t="s">
+        <v>23</v>
+      </c>
+      <c r="X20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1534,8 +2026,32 @@
       <c r="P21" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q21" t="s">
+        <v>23</v>
+      </c>
+      <c r="R21" t="s">
+        <v>23</v>
+      </c>
+      <c r="S21" t="s">
+        <v>23</v>
+      </c>
+      <c r="T21" t="s">
+        <v>23</v>
+      </c>
+      <c r="U21" t="s">
+        <v>23</v>
+      </c>
+      <c r="V21" t="s">
+        <v>23</v>
+      </c>
+      <c r="W21" t="s">
+        <v>23</v>
+      </c>
+      <c r="X21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1584,8 +2100,32 @@
       <c r="P22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q22" t="s">
+        <v>23</v>
+      </c>
+      <c r="R22" t="s">
+        <v>23</v>
+      </c>
+      <c r="S22" t="s">
+        <v>23</v>
+      </c>
+      <c r="T22" t="s">
+        <v>23</v>
+      </c>
+      <c r="U22" t="s">
+        <v>23</v>
+      </c>
+      <c r="V22" t="s">
+        <v>23</v>
+      </c>
+      <c r="W22" t="s">
+        <v>23</v>
+      </c>
+      <c r="X22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1634,8 +2174,32 @@
       <c r="P23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q23" t="s">
+        <v>23</v>
+      </c>
+      <c r="R23" t="s">
+        <v>23</v>
+      </c>
+      <c r="S23" t="s">
+        <v>23</v>
+      </c>
+      <c r="T23" t="s">
+        <v>23</v>
+      </c>
+      <c r="U23" t="s">
+        <v>23</v>
+      </c>
+      <c r="V23" t="s">
+        <v>23</v>
+      </c>
+      <c r="W23" t="s">
+        <v>23</v>
+      </c>
+      <c r="X23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1684,8 +2248,32 @@
       <c r="P24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q24" t="s">
+        <v>23</v>
+      </c>
+      <c r="R24" t="s">
+        <v>23</v>
+      </c>
+      <c r="S24" t="s">
+        <v>23</v>
+      </c>
+      <c r="T24" t="s">
+        <v>23</v>
+      </c>
+      <c r="U24" t="s">
+        <v>23</v>
+      </c>
+      <c r="V24" t="s">
+        <v>23</v>
+      </c>
+      <c r="W24" t="s">
+        <v>23</v>
+      </c>
+      <c r="X24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1734,8 +2322,32 @@
       <c r="P25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q25" t="s">
+        <v>23</v>
+      </c>
+      <c r="R25" t="s">
+        <v>23</v>
+      </c>
+      <c r="S25" t="s">
+        <v>23</v>
+      </c>
+      <c r="T25" t="s">
+        <v>23</v>
+      </c>
+      <c r="U25" t="s">
+        <v>23</v>
+      </c>
+      <c r="V25" t="s">
+        <v>23</v>
+      </c>
+      <c r="W25" t="s">
+        <v>23</v>
+      </c>
+      <c r="X25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1784,8 +2396,32 @@
       <c r="P26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q26" t="s">
+        <v>23</v>
+      </c>
+      <c r="R26" t="s">
+        <v>23</v>
+      </c>
+      <c r="S26" t="s">
+        <v>23</v>
+      </c>
+      <c r="T26" t="s">
+        <v>23</v>
+      </c>
+      <c r="U26" t="s">
+        <v>23</v>
+      </c>
+      <c r="V26" t="s">
+        <v>23</v>
+      </c>
+      <c r="W26" t="s">
+        <v>23</v>
+      </c>
+      <c r="X26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -1834,8 +2470,32 @@
       <c r="P27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q27" t="s">
+        <v>23</v>
+      </c>
+      <c r="R27" t="s">
+        <v>23</v>
+      </c>
+      <c r="S27" t="s">
+        <v>23</v>
+      </c>
+      <c r="T27" t="s">
+        <v>23</v>
+      </c>
+      <c r="U27" t="s">
+        <v>23</v>
+      </c>
+      <c r="V27" t="s">
+        <v>23</v>
+      </c>
+      <c r="W27" t="s">
+        <v>23</v>
+      </c>
+      <c r="X27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1884,8 +2544,32 @@
       <c r="P28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R28" t="s">
+        <v>23</v>
+      </c>
+      <c r="S28" t="s">
+        <v>23</v>
+      </c>
+      <c r="T28" t="s">
+        <v>23</v>
+      </c>
+      <c r="U28" t="s">
+        <v>23</v>
+      </c>
+      <c r="V28" t="s">
+        <v>23</v>
+      </c>
+      <c r="W28" t="s">
+        <v>23</v>
+      </c>
+      <c r="X28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1928,8 +2612,32 @@
       <c r="N29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O29" t="s">
+        <v>23</v>
+      </c>
+      <c r="P29" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>23</v>
+      </c>
+      <c r="R29" t="s">
+        <v>23</v>
+      </c>
+      <c r="S29" t="s">
+        <v>23</v>
+      </c>
+      <c r="T29" t="s">
+        <v>23</v>
+      </c>
+      <c r="U29" t="s">
+        <v>23</v>
+      </c>
+      <c r="V29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -1972,8 +2680,32 @@
       <c r="N30" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O30" t="s">
+        <v>23</v>
+      </c>
+      <c r="P30" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>23</v>
+      </c>
+      <c r="R30" t="s">
+        <v>23</v>
+      </c>
+      <c r="S30" t="s">
+        <v>23</v>
+      </c>
+      <c r="T30" t="s">
+        <v>23</v>
+      </c>
+      <c r="U30" t="s">
+        <v>23</v>
+      </c>
+      <c r="V30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -2016,8 +2748,32 @@
       <c r="N31" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O31" t="s">
+        <v>23</v>
+      </c>
+      <c r="P31" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>23</v>
+      </c>
+      <c r="R31" t="s">
+        <v>23</v>
+      </c>
+      <c r="S31" t="s">
+        <v>23</v>
+      </c>
+      <c r="T31" t="s">
+        <v>23</v>
+      </c>
+      <c r="U31" t="s">
+        <v>23</v>
+      </c>
+      <c r="V31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -2060,8 +2816,32 @@
       <c r="N32" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P32" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>23</v>
+      </c>
+      <c r="R32" t="s">
+        <v>23</v>
+      </c>
+      <c r="S32" t="s">
+        <v>23</v>
+      </c>
+      <c r="T32" t="s">
+        <v>23</v>
+      </c>
+      <c r="U32" t="s">
+        <v>23</v>
+      </c>
+      <c r="V32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -2104,8 +2884,32 @@
       <c r="N33" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O33" t="s">
+        <v>23</v>
+      </c>
+      <c r="P33" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>23</v>
+      </c>
+      <c r="R33" t="s">
+        <v>23</v>
+      </c>
+      <c r="S33" t="s">
+        <v>23</v>
+      </c>
+      <c r="T33" t="s">
+        <v>23</v>
+      </c>
+      <c r="U33" t="s">
+        <v>23</v>
+      </c>
+      <c r="V33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -2148,8 +2952,32 @@
       <c r="N34" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34" t="s">
+        <v>23</v>
+      </c>
+      <c r="P34" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>23</v>
+      </c>
+      <c r="R34" t="s">
+        <v>23</v>
+      </c>
+      <c r="S34" t="s">
+        <v>23</v>
+      </c>
+      <c r="T34" t="s">
+        <v>23</v>
+      </c>
+      <c r="U34" t="s">
+        <v>23</v>
+      </c>
+      <c r="V34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2192,8 +3020,32 @@
       <c r="N35" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35" t="s">
+        <v>23</v>
+      </c>
+      <c r="P35" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>23</v>
+      </c>
+      <c r="R35" t="s">
+        <v>23</v>
+      </c>
+      <c r="S35" t="s">
+        <v>23</v>
+      </c>
+      <c r="T35" t="s">
+        <v>23</v>
+      </c>
+      <c r="U35" t="s">
+        <v>23</v>
+      </c>
+      <c r="V35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2234,6 +3086,30 @@
         <v>23</v>
       </c>
       <c r="N36" t="s">
+        <v>23</v>
+      </c>
+      <c r="O36" t="s">
+        <v>23</v>
+      </c>
+      <c r="P36" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>23</v>
+      </c>
+      <c r="R36" t="s">
+        <v>23</v>
+      </c>
+      <c r="S36" t="s">
+        <v>23</v>
+      </c>
+      <c r="T36" t="s">
+        <v>23</v>
+      </c>
+      <c r="U36" t="s">
+        <v>23</v>
+      </c>
+      <c r="V36" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final set of survival and size data
</commit_message>
<xml_diff>
--- a/Data/raw_fecund_data.xlsx
+++ b/Data/raw_fecund_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/Lab_Projects/01_Small_projects/freshwater_choice/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B3C4ED-57E1-9A45-8976-C28CB2AC61EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF6C9E3-FC45-8D46-A55F-362B710CA456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{8320B239-817B-2D40-83A6-DE83587F0EE7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="32">
   <si>
     <t>exp_rep</t>
   </si>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8949BF81-7D7A-4643-97D8-DBE58FB94094}">
   <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="V29" sqref="V29:V36"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W29" sqref="W29:X36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2636,6 +2636,12 @@
       <c r="V29" t="s">
         <v>23</v>
       </c>
+      <c r="W29" t="s">
+        <v>23</v>
+      </c>
+      <c r="X29" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -2704,6 +2710,12 @@
       <c r="V30" t="s">
         <v>23</v>
       </c>
+      <c r="W30" t="s">
+        <v>23</v>
+      </c>
+      <c r="X30" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -2772,6 +2784,12 @@
       <c r="V31" t="s">
         <v>23</v>
       </c>
+      <c r="W31" t="s">
+        <v>23</v>
+      </c>
+      <c r="X31" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -2840,8 +2858,14 @@
       <c r="V32" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W32" t="s">
+        <v>23</v>
+      </c>
+      <c r="X32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -2908,8 +2932,14 @@
       <c r="V33" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W33" t="s">
+        <v>23</v>
+      </c>
+      <c r="X33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -2976,8 +3006,14 @@
       <c r="V34" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W34" t="s">
+        <v>23</v>
+      </c>
+      <c r="X34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -3044,8 +3080,14 @@
       <c r="V35" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W35" t="s">
+        <v>23</v>
+      </c>
+      <c r="X35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -3110,6 +3152,12 @@
         <v>23</v>
       </c>
       <c r="V36" t="s">
+        <v>23</v>
+      </c>
+      <c r="W36" t="s">
+        <v>23</v>
+      </c>
+      <c r="X36" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>